<commit_message>
Latest changes to NIM data breakdowns
</commit_message>
<xml_diff>
--- a/MATLAB/data/nim_data_dictionary.xlsx
+++ b/MATLAB/data/nim_data_dictionary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="income" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="111">
   <si>
     <t>Full Series Name</t>
   </si>
@@ -24,45 +24,18 @@
     <t>BA Code</t>
   </si>
   <si>
-    <t>Loans secured by 1-4 family residential properties</t>
-  </si>
-  <si>
-    <t>All other loans secured by real estate</t>
-  </si>
-  <si>
-    <t>Loans to finance agricultural production and other loans to farmers</t>
-  </si>
-  <si>
     <t>Call Report Code (RIAD)</t>
   </si>
   <si>
-    <t>Commercial and industrial loans</t>
-  </si>
-  <si>
-    <t>Credit card loans</t>
-  </si>
-  <si>
     <t>B485</t>
   </si>
   <si>
-    <t>Other (includes single payment, installment, student loans, and revolving credit plans other than credit cards</t>
-  </si>
-  <si>
     <t>B486</t>
   </si>
   <si>
-    <t>Loans to foreign governments and official institutions</t>
-  </si>
-  <si>
-    <t>All other loans in domestic offices</t>
-  </si>
-  <si>
     <t>B487</t>
   </si>
   <si>
-    <t>Interest and fee income on loans in foreign offices, Edge and Agreement subsidiaries, and IBFs</t>
-  </si>
-  <si>
     <t>Income from lease financing receivables</t>
   </si>
   <si>
@@ -144,15 +117,6 @@
     <t>flo11400</t>
   </si>
   <si>
-    <t>In foreign offices:</t>
-  </si>
-  <si>
-    <t>Interest and fee income on loans:</t>
-  </si>
-  <si>
-    <t>In domestic offices:</t>
-  </si>
-  <si>
     <t>flo10600</t>
   </si>
   <si>
@@ -174,12 +138,6 @@
     <t>Interest and dividend income on securities:</t>
   </si>
   <si>
-    <t>Loans to individuals for household, family, and other personal expenditures (i.e., consumer loans):</t>
-  </si>
-  <si>
-    <t>Loans Secured by Real Estate:</t>
-  </si>
-  <si>
     <t>flo12500</t>
   </si>
   <si>
@@ -207,9 +165,6 @@
     <t>Definition for 2001Q3 to Present different from definition for 1984Q3 to 2000Q4.</t>
   </si>
   <si>
-    <t>Total interest and fee income on loans (i.e., sum of above)</t>
-  </si>
-  <si>
     <t>Interest expense:</t>
   </si>
   <si>
@@ -352,6 +307,48 @@
   </si>
   <si>
     <t>cal91900</t>
+  </si>
+  <si>
+    <t>a. Interest and fee income on loans:</t>
+  </si>
+  <si>
+    <t>(1) In domestic offices:</t>
+  </si>
+  <si>
+    <t>(a) Loans Secured by Real Estate:</t>
+  </si>
+  <si>
+    <t>(1) Loans secured by 1-4 family residential properties</t>
+  </si>
+  <si>
+    <t>(2) All other loans secured by real estate</t>
+  </si>
+  <si>
+    <t>(b) Loans to finance agricultural production and other loans to farmers</t>
+  </si>
+  <si>
+    <t>© Commercial and industrial loans</t>
+  </si>
+  <si>
+    <t>(d) Loans to individuals for household, family, and other personal expenditures (i.e., consumer loans):</t>
+  </si>
+  <si>
+    <t>(1) Credit card loans</t>
+  </si>
+  <si>
+    <t>(2) Other (includes single payment, installment, student loans, and revolving credit plans other than credit cards</t>
+  </si>
+  <si>
+    <t>€ Loans to foreign governments and official institutions</t>
+  </si>
+  <si>
+    <t>(f) All other loans in domestic offices</t>
+  </si>
+  <si>
+    <t>(2) In foreign offices, Interest and fee income on loans in foreign offices, Edge and Agreement subsidiaries, and IBFs</t>
+  </si>
+  <si>
+    <t>(3) Total interest and fee income on loans (i.e., sum of above)</t>
   </si>
 </sst>
 </file>
@@ -432,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -449,6 +446,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -750,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,10 +784,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -777,21 +795,21 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -799,8 +817,8 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>44</v>
+      <c r="A4" s="16" t="s">
+        <v>98</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -808,122 +826,122 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>53</v>
+      <c r="A5" s="17" t="s">
+        <v>99</v>
       </c>
       <c r="B5" s="7">
         <v>4011</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
+      <c r="A6" s="18" t="s">
+        <v>100</v>
       </c>
       <c r="B6">
         <v>4435</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
+      <c r="A7" s="19" t="s">
+        <v>101</v>
       </c>
       <c r="B7" s="1">
         <v>4436</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>4</v>
+      <c r="A8" s="20" t="s">
+        <v>102</v>
       </c>
       <c r="B8" s="8">
         <v>4024</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>6</v>
+      <c r="A9" s="20" t="s">
+        <v>103</v>
       </c>
       <c r="B9" s="8">
         <v>4012</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>52</v>
+      <c r="A10" s="21" t="s">
+        <v>104</v>
       </c>
       <c r="B10" s="9">
         <v>4013</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>7</v>
+      <c r="A11" s="18" t="s">
+        <v>105</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>9</v>
+      <c r="A12" s="19" t="s">
+        <v>106</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>11</v>
+      <c r="A13" s="20" t="s">
+        <v>107</v>
       </c>
       <c r="B13" s="8">
         <v>4056</v>
@@ -932,183 +950,175 @@
         <v>11700</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>12</v>
+      <c r="A14" s="20" t="s">
+        <v>108</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>42</v>
+      <c r="A15" s="22" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16">
-        <v>4059</v>
+      <c r="A16" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B16" s="8">
+        <v>4010</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>63</v>
+        <v>6</v>
       </c>
       <c r="B17" s="8">
-        <v>4010</v>
+        <v>4065</v>
       </c>
       <c r="C17" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="8">
+        <v>4115</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="9">
+        <v>4218</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="12">
+        <v>4060</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="12"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="8">
+        <v>4069</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D23" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="8">
+        <v>4020</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="D24" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="8">
-        <v>4065</v>
-      </c>
-      <c r="C18" s="8" t="s">
+      <c r="B25" s="8">
+        <v>4518</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" s="8">
-        <v>4115</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" s="9">
-        <v>4218</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="11" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="12">
-        <v>4060</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E23" s="12"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="8">
-        <v>4069</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="8">
-        <v>4020</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="8">
-        <v>4518</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>49</v>
+      <c r="D25" s="10" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1136,10 +1146,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1147,31 +1157,31 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1180,80 +1190,80 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B6">
         <v>4508</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B8">
         <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="E9" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="B11" s="5">
         <v>4172</v>
@@ -1264,72 +1274,72 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B12" s="8">
         <v>4180</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="B13" s="8">
         <v>4185</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="B14" s="8">
         <v>4200</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="B15">
         <v>4073</v>
       </c>
       <c r="C15" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="D15" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="B16">
         <v>4074</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1342,8 +1352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,10 +1366,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1367,94 +1377,94 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="B4">
         <v>3381</v>
       </c>
       <c r="C4" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B5">
         <v>8641</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="D5" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="B6">
         <v>3365</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="B7" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="C7" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="D7" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B8">
         <v>3401</v>
       </c>
       <c r="C8" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="D8" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Put together data for analysis of NIMs constructed with and without trading assets and based on rankings of total assets and just total interest-earning assets.
</commit_message>
<xml_diff>
--- a/MATLAB/data/nim_data_dictionary.xlsx
+++ b/MATLAB/data/nim_data_dictionary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
+    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="income" sheetId="1" r:id="rId1"/>
@@ -165,51 +165,12 @@
     <t>Definition for 2001Q3 to Present different from definition for 1984Q3 to 2000Q4.</t>
   </si>
   <si>
-    <t>Interest expense:</t>
-  </si>
-  <si>
-    <t>Interest on deposits:</t>
-  </si>
-  <si>
-    <t>Interest on deposits in domestic offices:</t>
-  </si>
-  <si>
-    <t>Transaction accounts (interest-bearing demand deposits, NOW accounts, ATS accounts, and telephone and preauthorized transfer accounts)</t>
-  </si>
-  <si>
-    <t>Nontransaction accounts:</t>
-  </si>
-  <si>
-    <t>Savings deposits (includes MMDAs)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time deposits of $100,000 or more </t>
-  </si>
-  <si>
     <t>A517</t>
   </si>
   <si>
-    <t>Time deposits of less than $100,000</t>
-  </si>
-  <si>
     <t>A518</t>
   </si>
   <si>
-    <t>Interest on deposits in foreign offices, Edge and Agreement subsidiaries, and IBFs</t>
-  </si>
-  <si>
-    <t>Expense of federal funds purchased and securities sold under agreements to repurchase</t>
-  </si>
-  <si>
-    <t>Interest on trading liabilities and other borrowed money</t>
-  </si>
-  <si>
-    <t>Interest on subordinated notes and debentures</t>
-  </si>
-  <si>
-    <t>Total interest expense</t>
-  </si>
-  <si>
     <t>Net interest income</t>
   </si>
   <si>
@@ -225,9 +186,6 @@
     <t>flo15700</t>
   </si>
   <si>
-    <t>1987Q3 to Present</t>
-  </si>
-  <si>
     <t>flo15800</t>
   </si>
   <si>
@@ -349,6 +307,48 @@
   </si>
   <si>
     <t>(3) Total interest and fee income on loans (i.e., sum of above)</t>
+  </si>
+  <si>
+    <t>2. Interest expense:</t>
+  </si>
+  <si>
+    <t>a. Interest on deposits:</t>
+  </si>
+  <si>
+    <t>(1) Interest on deposits in domestic offices:</t>
+  </si>
+  <si>
+    <t>(a) Transaction accounts (interest-bearing demand deposits, NOW accounts, ATS accounts, and telephone and preauthorized transfer accounts)</t>
+  </si>
+  <si>
+    <t>(b) Nontransaction accounts:</t>
+  </si>
+  <si>
+    <t>(1) Savings deposits (includes MMDAs)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(2) Time deposits of $100,000 or more </t>
+  </si>
+  <si>
+    <t>(3) Time deposits of less than $100,000</t>
+  </si>
+  <si>
+    <t>b. Expense of federal funds purchased and securities sold under agreements to repurchase</t>
+  </si>
+  <si>
+    <t>c. Interest on trading liabilities and other borrowed money</t>
+  </si>
+  <si>
+    <t>d. Interest on subordinated notes and debentures</t>
+  </si>
+  <si>
+    <t>e. Total interest expense</t>
+  </si>
+  <si>
+    <t>(2) Interest on deposits in foreign offices, Edge and Agreement subsidiaries, and IBFs</t>
+  </si>
+  <si>
+    <t>1987Q1 to Present</t>
   </si>
 </sst>
 </file>
@@ -429,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -444,8 +444,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -466,6 +464,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -770,8 +786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A3" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,7 +803,7 @@
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -809,7 +825,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -817,8 +833,8 @@
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
-        <v>98</v>
+      <c r="A4" s="14" t="s">
+        <v>84</v>
       </c>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -826,8 +842,8 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
-        <v>99</v>
+      <c r="A5" s="15" t="s">
+        <v>85</v>
       </c>
       <c r="B5" s="7">
         <v>4011</v>
@@ -841,8 +857,8 @@
       <c r="E5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>100</v>
+      <c r="A6" s="16" t="s">
+        <v>86</v>
       </c>
       <c r="B6">
         <v>4435</v>
@@ -855,8 +871,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>101</v>
+      <c r="A7" s="17" t="s">
+        <v>87</v>
       </c>
       <c r="B7" s="1">
         <v>4436</v>
@@ -870,8 +886,8 @@
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
-        <v>102</v>
+      <c r="A8" s="18" t="s">
+        <v>88</v>
       </c>
       <c r="B8" s="8">
         <v>4024</v>
@@ -884,8 +900,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>103</v>
+      <c r="A9" s="18" t="s">
+        <v>89</v>
       </c>
       <c r="B9" s="8">
         <v>4012</v>
@@ -898,8 +914,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
-        <v>104</v>
+      <c r="A10" s="19" t="s">
+        <v>90</v>
       </c>
       <c r="B10" s="9">
         <v>4013</v>
@@ -912,8 +928,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>105</v>
+      <c r="A11" s="16" t="s">
+        <v>91</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -926,8 +942,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>106</v>
+      <c r="A12" s="17" t="s">
+        <v>92</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>4</v>
@@ -940,8 +956,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
-        <v>107</v>
+      <c r="A13" s="18" t="s">
+        <v>93</v>
       </c>
       <c r="B13" s="8">
         <v>4056</v>
@@ -954,8 +970,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>108</v>
+      <c r="A14" s="18" t="s">
+        <v>94</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>5</v>
@@ -971,13 +987,13 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
-        <v>109</v>
+      <c r="A15" s="20" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="B16" s="8">
         <v>4010</v>
@@ -1131,8 +1147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,7 +1165,7 @@
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1171,17 +1187,17 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>49</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>50</v>
+      <c r="A4" s="21" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
-        <v>51</v>
+      <c r="A5" s="19" t="s">
+        <v>99</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1189,154 +1205,154 @@
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>52</v>
+      <c r="A6" s="22" t="s">
+        <v>100</v>
       </c>
       <c r="B6">
         <v>4508</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>69</v>
+      <c r="A7" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>110</v>
       </c>
       <c r="E7" s="9"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>54</v>
+      <c r="A8" s="24" t="s">
+        <v>102</v>
       </c>
       <c r="B8">
         <v>93</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>55</v>
+      <c r="A9" s="24" t="s">
+        <v>103</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>57</v>
+      <c r="A10" s="25" t="s">
+        <v>104</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="E10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="5">
+      <c r="A11" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B11" s="7">
         <v>4172</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>60</v>
+      <c r="A12" s="21" t="s">
+        <v>105</v>
       </c>
       <c r="B12" s="8">
         <v>4180</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>61</v>
+      <c r="A13" s="21" t="s">
+        <v>106</v>
       </c>
       <c r="B13" s="8">
         <v>4185</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>62</v>
+      <c r="A14" s="21" t="s">
+        <v>107</v>
       </c>
       <c r="B14" s="8">
         <v>4200</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>63</v>
+      <c r="A15" s="23" t="s">
+        <v>108</v>
       </c>
       <c r="B15">
         <v>4073</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B16">
         <v>4074</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="D16" t="s">
         <v>22</v>
@@ -1352,8 +1368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1369,7 +1385,7 @@
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1377,7 +1393,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
@@ -1388,10 +1404,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
         <v>22</v>
@@ -1399,13 +1415,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B4">
         <v>3381</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
         <v>22</v>
@@ -1413,27 +1429,27 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="B5">
         <v>8641</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B6">
         <v>3365</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="D6" t="s">
         <v>22</v>
@@ -1441,30 +1457,30 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="D7" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="B8">
         <v>3401</v>
       </c>
       <c r="C8" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="D8" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>